<commit_message>
Updated files for draft with 36 states and 640 districts (2015 boundaries)
</commit_message>
<xml_diff>
--- a/data/mapping_ext.xlsx
+++ b/data/mapping_ext.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs-child-malnutrition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF344E5-C1BB-466C-A406-D2013A63AAC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25050" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nfhs5_state" sheetId="1" r:id="rId1"/>
@@ -17,15 +18,17 @@
     <sheet name="nfhs4_state" sheetId="3" r:id="rId3"/>
     <sheet name="nfhs4_district" sheetId="4" r:id="rId4"/>
     <sheet name="labels" sheetId="5" r:id="rId5"/>
+    <sheet name="ncm_variables" sheetId="6" r:id="rId6"/>
+    <sheet name="v024" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">nfhs4_state!$A$1:$B$115</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nfhs5_state!$B$1:$C$132</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="811">
   <si>
     <t>ID</t>
   </si>
@@ -1697,14 +1700,793 @@
   </si>
   <si>
     <t>Remark added on district formation</t>
+  </si>
+  <si>
+    <t>iair52dt</t>
+  </si>
+  <si>
+    <t>iair74dt</t>
+  </si>
+  <si>
+    <t>iair7adt</t>
+  </si>
+  <si>
+    <t>iahr52dt</t>
+  </si>
+  <si>
+    <t>iahr74dt</t>
+  </si>
+  <si>
+    <t>iahr7adt</t>
+  </si>
+  <si>
+    <t>iapr52dt</t>
+  </si>
+  <si>
+    <t>iapr74dt</t>
+  </si>
+  <si>
+    <t>iapr7adt</t>
+  </si>
+  <si>
+    <t>v021</t>
+  </si>
+  <si>
+    <t>iapr52dt_child</t>
+  </si>
+  <si>
+    <t>iapr74dt_child</t>
+  </si>
+  <si>
+    <t>iapr7adt_child</t>
+  </si>
+  <si>
+    <t>hv001</t>
+  </si>
+  <si>
+    <t>hv005</t>
+  </si>
+  <si>
+    <t>hv021</t>
+  </si>
+  <si>
+    <t>hc1</t>
+  </si>
+  <si>
+    <t>hc56</t>
+  </si>
+  <si>
+    <t>hc27</t>
+  </si>
+  <si>
+    <t>hv024</t>
+  </si>
+  <si>
+    <t>hv025</t>
+  </si>
+  <si>
+    <t>hv270</t>
+  </si>
+  <si>
+    <t>hc70</t>
+  </si>
+  <si>
+    <t>hc71</t>
+  </si>
+  <si>
+    <t>hc72</t>
+  </si>
+  <si>
+    <t>WHZ</t>
+  </si>
+  <si>
+    <t>WAZ</t>
+  </si>
+  <si>
+    <t>HAZ</t>
+  </si>
+  <si>
+    <t>Age in months</t>
+  </si>
+  <si>
+    <t>Hemoglobin</t>
+  </si>
+  <si>
+    <t>Sex (1 = Male, 2 = Female)</t>
+  </si>
+  <si>
+    <t>PSU number</t>
+  </si>
+  <si>
+    <t>National HH weight</t>
+  </si>
+  <si>
+    <t>PSU (same as SH021)</t>
+  </si>
+  <si>
+    <t>hv022</t>
+  </si>
+  <si>
+    <t>Stratum</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Residence (1 = Urban, 2 = Rural)</t>
+  </si>
+  <si>
+    <t>Wealth index</t>
+  </si>
+  <si>
+    <t>Number of members</t>
+  </si>
+  <si>
+    <t>v133</t>
+  </si>
+  <si>
+    <t>v155</t>
+  </si>
+  <si>
+    <t>v511</t>
+  </si>
+  <si>
+    <t>v445</t>
+  </si>
+  <si>
+    <t>v463z</t>
+  </si>
+  <si>
+    <t>s569</t>
+  </si>
+  <si>
+    <t>v456</t>
+  </si>
+  <si>
+    <t>v001</t>
+  </si>
+  <si>
+    <t>v005</t>
+  </si>
+  <si>
+    <t>v022</t>
+  </si>
+  <si>
+    <t>v024</t>
+  </si>
+  <si>
+    <t>v025</t>
+  </si>
+  <si>
+    <t>Education in single years</t>
+  </si>
+  <si>
+    <t>Literacy</t>
+  </si>
+  <si>
+    <t>Age at first cohabitation</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>v454</t>
+  </si>
+  <si>
+    <t>Hb adjusted for altitude and smoking</t>
+  </si>
+  <si>
+    <t>Drinks alcohol (0 = No, 1 = Yes)</t>
+  </si>
+  <si>
+    <t>Does not use tobacco (0 = No, 1 = Yes/nothing)</t>
+  </si>
+  <si>
+    <t>s716</t>
+  </si>
+  <si>
+    <t>v190</t>
+  </si>
+  <si>
+    <t>Currently pregnant (0 = No/DK, 1 = Yes, 9 = Miss)</t>
+  </si>
+  <si>
+    <t>s720</t>
+  </si>
+  <si>
+    <t>Member of house covered by a health scheme</t>
+  </si>
+  <si>
+    <t>sh64</t>
+  </si>
+  <si>
+    <t>Type of cooking fuel</t>
+  </si>
+  <si>
+    <t>hv226</t>
+  </si>
+  <si>
+    <t>sh71</t>
+  </si>
+  <si>
+    <t>sh54</t>
+  </si>
+  <si>
+    <t>Household number</t>
+  </si>
+  <si>
+    <t>hv002</t>
+  </si>
+  <si>
+    <t>v002</t>
+  </si>
+  <si>
+    <t>hv201</t>
+  </si>
+  <si>
+    <t>hv205</t>
+  </si>
+  <si>
+    <t>hv225</t>
+  </si>
+  <si>
+    <t>hv206</t>
+  </si>
+  <si>
+    <t>hv012</t>
+  </si>
+  <si>
+    <t>Source of drinking water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of toilet facility </t>
+  </si>
+  <si>
+    <t>Has electricity (0 = No, 1 = Yes)</t>
+  </si>
+  <si>
+    <t>Share toilet with other households (0 = No, 1 = Yes)</t>
+  </si>
+  <si>
+    <t>new_var</t>
+  </si>
+  <si>
+    <t>psu</t>
+  </si>
+  <si>
+    <t>stratum</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>residence</t>
+  </si>
+  <si>
+    <t>wealth</t>
+  </si>
+  <si>
+    <t>hhno</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>psu2</t>
+  </si>
+  <si>
+    <t>c_age</t>
+  </si>
+  <si>
+    <t>c_sex</t>
+  </si>
+  <si>
+    <t>c_haz</t>
+  </si>
+  <si>
+    <t>c_waz</t>
+  </si>
+  <si>
+    <t>c_whz</t>
+  </si>
+  <si>
+    <t>c_hb</t>
+  </si>
+  <si>
+    <t>m_literacy</t>
+  </si>
+  <si>
+    <t>m_eduyr</t>
+  </si>
+  <si>
+    <t>m_cohabitation</t>
+  </si>
+  <si>
+    <t>m_bmi</t>
+  </si>
+  <si>
+    <t>m_pregnant</t>
+  </si>
+  <si>
+    <t>m_hb</t>
+  </si>
+  <si>
+    <t>m_notobacco</t>
+  </si>
+  <si>
+    <t>m_alcohol</t>
+  </si>
+  <si>
+    <t>m_insurance</t>
+  </si>
+  <si>
+    <t>m_fuel</t>
+  </si>
+  <si>
+    <t>m_water</t>
+  </si>
+  <si>
+    <t>m_toilet</t>
+  </si>
+  <si>
+    <t>m_electricity</t>
+  </si>
+  <si>
+    <t>m_sharetoilet</t>
+  </si>
+  <si>
+    <t>m_nmembers</t>
+  </si>
+  <si>
+    <t>v024_nfhs3</t>
+  </si>
+  <si>
+    <t>andaman and nicobar islands</t>
+  </si>
+  <si>
+    <t>Andaman &amp; Nicobar Islands</t>
+  </si>
+  <si>
+    <t>andhra pradesh</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>arunachal pradesh</t>
+  </si>
+  <si>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>assam</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>bihar</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>chandigarh</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>chhattisgarh</t>
+  </si>
+  <si>
+    <t>Chhattisgarh</t>
+  </si>
+  <si>
+    <t>daman and diu</t>
+  </si>
+  <si>
+    <t>goa</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>gujarat</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>haryana</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>himachal pradesh</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>jammu and kashmir</t>
+  </si>
+  <si>
+    <t>Jammu &amp; Kashmir</t>
+  </si>
+  <si>
+    <t>jharkhand</t>
+  </si>
+  <si>
+    <t>Jharkhand</t>
+  </si>
+  <si>
+    <t>karnataka</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>kerala</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>ladakh</t>
+  </si>
+  <si>
+    <t>lakshadweep</t>
+  </si>
+  <si>
+    <t>Lakshadweep</t>
+  </si>
+  <si>
+    <t>madhya pradesh</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>maharashtra</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>manipur</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>meghalaya</t>
+  </si>
+  <si>
+    <t>Meghalaya</t>
+  </si>
+  <si>
+    <t>mizoram</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
+  </si>
+  <si>
+    <t>nagaland</t>
+  </si>
+  <si>
+    <t>Nagaland</t>
+  </si>
+  <si>
+    <t>delhi</t>
+  </si>
+  <si>
+    <t>NCT of Delhi</t>
+  </si>
+  <si>
+    <t>odisha</t>
+  </si>
+  <si>
+    <t>Odisha</t>
+  </si>
+  <si>
+    <t>orissa</t>
+  </si>
+  <si>
+    <t>puducherry</t>
+  </si>
+  <si>
+    <t>Puducherry</t>
+  </si>
+  <si>
+    <t>punjab</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>rajasthan</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>sikkim</t>
+  </si>
+  <si>
+    <t>Sikkim</t>
+  </si>
+  <si>
+    <t>tamil nadu</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>telangana</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>tripura</t>
+  </si>
+  <si>
+    <t>Tripura</t>
+  </si>
+  <si>
+    <t>uttar pradesh</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>uttarakhand</t>
+  </si>
+  <si>
+    <t>Uttarakhand</t>
+  </si>
+  <si>
+    <t>uttaranchal</t>
+  </si>
+  <si>
+    <t>west bengal</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>v024_nfhs5</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>Dadra &amp; Nagar Haveli</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>Daman &amp; Diu</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>GJ</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>JK</t>
+  </si>
+  <si>
+    <t>KA</t>
+  </si>
+  <si>
+    <t>KL</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MZ</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>JH</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>v024_nfhs4</t>
+  </si>
+  <si>
+    <t>dadra and nagar haveli</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>statecode</t>
+  </si>
+  <si>
+    <t>Create from district data into DN</t>
+  </si>
+  <si>
+    <t>Create from district data into DD</t>
+  </si>
+  <si>
+    <t>Combine JK and LH before summarizing into JK</t>
+  </si>
+  <si>
+    <t>comment for NFHS5</t>
+  </si>
+  <si>
+    <t>comment for NFHS3</t>
+  </si>
+  <si>
+    <t>rbind rows for AP after renaming into TG</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>sdist</t>
+  </si>
+  <si>
+    <t>sdistri</t>
+  </si>
+  <si>
+    <t>shdist</t>
+  </si>
+  <si>
+    <t>shdistri</t>
+  </si>
+  <si>
+    <t>jammu &amp; kashmir</t>
+  </si>
+  <si>
+    <t>andaman &amp; nicobar islands</t>
+  </si>
+  <si>
+    <t>Age of respondent</t>
+  </si>
+  <si>
+    <t>v012</t>
+  </si>
+  <si>
+    <t>m_age</t>
+  </si>
+  <si>
+    <t>ha1</t>
+  </si>
+  <si>
+    <t>iabr52dt</t>
+  </si>
+  <si>
+    <t>iabr74dt</t>
+  </si>
+  <si>
+    <t>iabr7adt</t>
+  </si>
+  <si>
+    <t>Date of interview</t>
+  </si>
+  <si>
+    <t>v008</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>m_interview</t>
+  </si>
+  <si>
+    <t>c_dob</t>
+  </si>
+  <si>
+    <t>nct of delhi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1738,9 +2520,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1764,11 +2550,13 @@
     <sheetNames>
       <sheetName val="extracted indicators-editing"/>
       <sheetName val="states"/>
-      <sheetName val="nfhs5_sample"/>
       <sheetName val="nfhs_1"/>
       <sheetName val="nfhs_2"/>
       <sheetName val="nfhs_3"/>
       <sheetName val="nfhs_4"/>
+      <sheetName val="nfhs5_sample"/>
+      <sheetName val="nfhs5_factsheet_map"/>
+      <sheetName val="nfhs_4d"/>
       <sheetName val="indicator_map"/>
       <sheetName val="dist_mapping"/>
       <sheetName val="nfhs5_state"/>
@@ -1785,7 +2573,9 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
-      <sheetData sheetId="7">
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
         <row r="2">
           <cell r="B2" t="str">
             <v>Population (female) age 6 years and above who ever attended school (%)</v>
@@ -2252,12 +3042,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="11">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>S01</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2525,11 +3321,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3995,7 +4791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0"/>
@@ -5166,7 +5962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0"/>
@@ -6875,13 +7671,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B115"/>
+  <autoFilter ref="A1:B115" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0"/>
@@ -7931,7 +8727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8296,4 +9092,1626 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF69C584-A901-4755-AAF5-5F5002664C77}">
+  <dimension ref="A1:Q34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B2" t="s">
+        <v>637</v>
+      </c>
+      <c r="C2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F2" t="s">
+        <v>601</v>
+      </c>
+      <c r="G2" t="s">
+        <v>601</v>
+      </c>
+      <c r="H2" t="s">
+        <v>601</v>
+      </c>
+      <c r="I2" t="s">
+        <v>567</v>
+      </c>
+      <c r="J2" t="s">
+        <v>567</v>
+      </c>
+      <c r="K2" t="s">
+        <v>567</v>
+      </c>
+      <c r="L2" t="s">
+        <v>567</v>
+      </c>
+      <c r="M2" t="s">
+        <v>567</v>
+      </c>
+      <c r="N2" t="s">
+        <v>567</v>
+      </c>
+      <c r="O2" t="s">
+        <v>601</v>
+      </c>
+      <c r="P2" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>624</v>
+      </c>
+      <c r="B3" t="s">
+        <v>642</v>
+      </c>
+      <c r="C3" t="s">
+        <v>625</v>
+      </c>
+      <c r="D3" t="s">
+        <v>625</v>
+      </c>
+      <c r="E3" t="s">
+        <v>625</v>
+      </c>
+      <c r="F3" t="s">
+        <v>626</v>
+      </c>
+      <c r="G3" t="s">
+        <v>626</v>
+      </c>
+      <c r="H3" t="s">
+        <v>626</v>
+      </c>
+      <c r="I3" t="s">
+        <v>625</v>
+      </c>
+      <c r="J3" t="s">
+        <v>625</v>
+      </c>
+      <c r="K3" t="s">
+        <v>625</v>
+      </c>
+      <c r="L3" t="s">
+        <v>625</v>
+      </c>
+      <c r="M3" t="s">
+        <v>625</v>
+      </c>
+      <c r="N3" t="s">
+        <v>625</v>
+      </c>
+      <c r="O3" t="s">
+        <v>626</v>
+      </c>
+      <c r="P3" t="s">
+        <v>626</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B4" t="s">
+        <v>643</v>
+      </c>
+      <c r="C4" t="s">
+        <v>568</v>
+      </c>
+      <c r="D4" t="s">
+        <v>568</v>
+      </c>
+      <c r="E4" t="s">
+        <v>568</v>
+      </c>
+      <c r="F4" t="s">
+        <v>602</v>
+      </c>
+      <c r="G4" t="s">
+        <v>602</v>
+      </c>
+      <c r="H4" t="s">
+        <v>602</v>
+      </c>
+      <c r="I4" t="s">
+        <v>568</v>
+      </c>
+      <c r="J4" t="s">
+        <v>568</v>
+      </c>
+      <c r="K4" t="s">
+        <v>568</v>
+      </c>
+      <c r="L4" t="s">
+        <v>568</v>
+      </c>
+      <c r="M4" t="s">
+        <v>568</v>
+      </c>
+      <c r="N4" t="s">
+        <v>568</v>
+      </c>
+      <c r="O4" t="s">
+        <v>602</v>
+      </c>
+      <c r="P4" t="s">
+        <v>602</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>587</v>
+      </c>
+      <c r="B5" t="s">
+        <v>644</v>
+      </c>
+      <c r="C5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D5" t="s">
+        <v>569</v>
+      </c>
+      <c r="E5" t="s">
+        <v>569</v>
+      </c>
+      <c r="F5" t="s">
+        <v>563</v>
+      </c>
+      <c r="G5" t="s">
+        <v>563</v>
+      </c>
+      <c r="H5" t="s">
+        <v>563</v>
+      </c>
+      <c r="I5" t="s">
+        <v>569</v>
+      </c>
+      <c r="J5" t="s">
+        <v>569</v>
+      </c>
+      <c r="K5" t="s">
+        <v>569</v>
+      </c>
+      <c r="L5" t="s">
+        <v>569</v>
+      </c>
+      <c r="M5" t="s">
+        <v>569</v>
+      </c>
+      <c r="N5" t="s">
+        <v>569</v>
+      </c>
+      <c r="O5" t="s">
+        <v>563</v>
+      </c>
+      <c r="P5" t="s">
+        <v>563</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B6" t="s">
+        <v>638</v>
+      </c>
+      <c r="C6" t="s">
+        <v>588</v>
+      </c>
+      <c r="D6" t="s">
+        <v>588</v>
+      </c>
+      <c r="E6" t="s">
+        <v>588</v>
+      </c>
+      <c r="F6" t="s">
+        <v>603</v>
+      </c>
+      <c r="G6" t="s">
+        <v>603</v>
+      </c>
+      <c r="H6" t="s">
+        <v>603</v>
+      </c>
+      <c r="I6" t="s">
+        <v>588</v>
+      </c>
+      <c r="J6" t="s">
+        <v>588</v>
+      </c>
+      <c r="K6" t="s">
+        <v>588</v>
+      </c>
+      <c r="L6" t="s">
+        <v>588</v>
+      </c>
+      <c r="M6" t="s">
+        <v>588</v>
+      </c>
+      <c r="N6" t="s">
+        <v>588</v>
+      </c>
+      <c r="O6" t="s">
+        <v>603</v>
+      </c>
+      <c r="P6" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>590</v>
+      </c>
+      <c r="B7" t="s">
+        <v>639</v>
+      </c>
+      <c r="C7" t="s">
+        <v>573</v>
+      </c>
+      <c r="D7" t="s">
+        <v>573</v>
+      </c>
+      <c r="E7" t="s">
+        <v>573</v>
+      </c>
+      <c r="F7" t="s">
+        <v>604</v>
+      </c>
+      <c r="G7" t="s">
+        <v>604</v>
+      </c>
+      <c r="H7" t="s">
+        <v>604</v>
+      </c>
+      <c r="I7" t="s">
+        <v>573</v>
+      </c>
+      <c r="J7" t="s">
+        <v>573</v>
+      </c>
+      <c r="K7" t="s">
+        <v>573</v>
+      </c>
+      <c r="L7" t="s">
+        <v>573</v>
+      </c>
+      <c r="M7" t="s">
+        <v>573</v>
+      </c>
+      <c r="N7" t="s">
+        <v>573</v>
+      </c>
+      <c r="O7" t="s">
+        <v>604</v>
+      </c>
+      <c r="P7" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>788</v>
+      </c>
+      <c r="B8" t="s">
+        <v>789</v>
+      </c>
+      <c r="D8" t="s">
+        <v>793</v>
+      </c>
+      <c r="E8" t="s">
+        <v>792</v>
+      </c>
+      <c r="G8" t="s">
+        <v>791</v>
+      </c>
+      <c r="H8" t="s">
+        <v>790</v>
+      </c>
+      <c r="J8" t="s">
+        <v>793</v>
+      </c>
+      <c r="K8" t="s">
+        <v>792</v>
+      </c>
+      <c r="M8" t="s">
+        <v>793</v>
+      </c>
+      <c r="N8" t="s">
+        <v>792</v>
+      </c>
+      <c r="P8" t="s">
+        <v>791</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>591</v>
+      </c>
+      <c r="B9" t="s">
+        <v>640</v>
+      </c>
+      <c r="C9" t="s">
+        <v>574</v>
+      </c>
+      <c r="D9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E9" t="s">
+        <v>574</v>
+      </c>
+      <c r="F9" t="s">
+        <v>605</v>
+      </c>
+      <c r="G9" t="s">
+        <v>605</v>
+      </c>
+      <c r="H9" t="s">
+        <v>605</v>
+      </c>
+      <c r="I9" t="s">
+        <v>574</v>
+      </c>
+      <c r="J9" t="s">
+        <v>574</v>
+      </c>
+      <c r="K9" t="s">
+        <v>574</v>
+      </c>
+      <c r="L9" t="s">
+        <v>574</v>
+      </c>
+      <c r="M9" t="s">
+        <v>574</v>
+      </c>
+      <c r="N9" t="s">
+        <v>574</v>
+      </c>
+      <c r="O9" t="s">
+        <v>605</v>
+      </c>
+      <c r="P9" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>592</v>
+      </c>
+      <c r="B10" t="s">
+        <v>641</v>
+      </c>
+      <c r="C10" t="s">
+        <v>575</v>
+      </c>
+      <c r="D10" t="s">
+        <v>575</v>
+      </c>
+      <c r="E10" t="s">
+        <v>575</v>
+      </c>
+      <c r="F10" t="s">
+        <v>615</v>
+      </c>
+      <c r="G10" t="s">
+        <v>615</v>
+      </c>
+      <c r="H10" t="s">
+        <v>615</v>
+      </c>
+      <c r="I10" t="s">
+        <v>575</v>
+      </c>
+      <c r="J10" t="s">
+        <v>575</v>
+      </c>
+      <c r="K10" t="s">
+        <v>575</v>
+      </c>
+      <c r="L10" t="s">
+        <v>575</v>
+      </c>
+      <c r="M10" t="s">
+        <v>575</v>
+      </c>
+      <c r="N10" t="s">
+        <v>575</v>
+      </c>
+      <c r="O10" t="s">
+        <v>615</v>
+      </c>
+      <c r="P10" t="s">
+        <v>615</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>582</v>
+      </c>
+      <c r="B11" t="s">
+        <v>645</v>
+      </c>
+      <c r="C11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D11" t="s">
+        <v>570</v>
+      </c>
+      <c r="E11" t="s">
+        <v>570</v>
+      </c>
+      <c r="L11" t="s">
+        <v>799</v>
+      </c>
+      <c r="M11" t="s">
+        <v>799</v>
+      </c>
+      <c r="N11" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>584</v>
+      </c>
+      <c r="B12" t="s">
+        <v>646</v>
+      </c>
+      <c r="C12" t="s">
+        <v>572</v>
+      </c>
+      <c r="D12" t="s">
+        <v>572</v>
+      </c>
+      <c r="E12" t="s">
+        <v>572</v>
+      </c>
+      <c r="O12" t="s">
+        <v>807</v>
+      </c>
+      <c r="P12" t="s">
+        <v>807</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>583</v>
+      </c>
+      <c r="B13" t="s">
+        <v>650</v>
+      </c>
+      <c r="C13" t="s">
+        <v>571</v>
+      </c>
+      <c r="D13" t="s">
+        <v>571</v>
+      </c>
+      <c r="E13" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>581</v>
+      </c>
+      <c r="B14" t="s">
+        <v>647</v>
+      </c>
+      <c r="C14" t="s">
+        <v>576</v>
+      </c>
+      <c r="D14" t="s">
+        <v>576</v>
+      </c>
+      <c r="E14" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>580</v>
+      </c>
+      <c r="B15" t="s">
+        <v>648</v>
+      </c>
+      <c r="C15" t="s">
+        <v>577</v>
+      </c>
+      <c r="D15" t="s">
+        <v>577</v>
+      </c>
+      <c r="E15" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>579</v>
+      </c>
+      <c r="B16" t="s">
+        <v>649</v>
+      </c>
+      <c r="C16" t="s">
+        <v>578</v>
+      </c>
+      <c r="D16" t="s">
+        <v>578</v>
+      </c>
+      <c r="E16" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>796</v>
+      </c>
+      <c r="B17" t="s">
+        <v>798</v>
+      </c>
+      <c r="F17" t="s">
+        <v>797</v>
+      </c>
+      <c r="G17" t="s">
+        <v>797</v>
+      </c>
+      <c r="H17" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>606</v>
+      </c>
+      <c r="B18" t="s">
+        <v>652</v>
+      </c>
+      <c r="F18" t="s">
+        <v>594</v>
+      </c>
+      <c r="G18" t="s">
+        <v>594</v>
+      </c>
+      <c r="H18" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>607</v>
+      </c>
+      <c r="B19" t="s">
+        <v>651</v>
+      </c>
+      <c r="F19" t="s">
+        <v>595</v>
+      </c>
+      <c r="G19" t="s">
+        <v>595</v>
+      </c>
+      <c r="H19" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>608</v>
+      </c>
+      <c r="B20" t="s">
+        <v>653</v>
+      </c>
+      <c r="F20" t="s">
+        <v>596</v>
+      </c>
+      <c r="G20" t="s">
+        <v>596</v>
+      </c>
+      <c r="H20" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>609</v>
+      </c>
+      <c r="B21" t="s">
+        <v>654</v>
+      </c>
+      <c r="F21" t="s">
+        <v>597</v>
+      </c>
+      <c r="G21" t="s">
+        <v>597</v>
+      </c>
+      <c r="H21" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>616</v>
+      </c>
+      <c r="B22" t="s">
+        <v>655</v>
+      </c>
+      <c r="F22" t="s">
+        <v>610</v>
+      </c>
+      <c r="G22" t="s">
+        <v>610</v>
+      </c>
+      <c r="H22" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>611</v>
+      </c>
+      <c r="B23" t="s">
+        <v>656</v>
+      </c>
+      <c r="F23" t="s">
+        <v>600</v>
+      </c>
+      <c r="G23" t="s">
+        <v>600</v>
+      </c>
+      <c r="H23" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>613</v>
+      </c>
+      <c r="B24" t="s">
+        <v>657</v>
+      </c>
+      <c r="F24" t="s">
+        <v>598</v>
+      </c>
+      <c r="G24" t="s">
+        <v>598</v>
+      </c>
+      <c r="H24" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>612</v>
+      </c>
+      <c r="B25" t="s">
+        <v>658</v>
+      </c>
+      <c r="F25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G25" t="s">
+        <v>614</v>
+      </c>
+      <c r="H25" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>618</v>
+      </c>
+      <c r="B26" t="s">
+        <v>659</v>
+      </c>
+      <c r="I26" t="s">
+        <v>619</v>
+      </c>
+      <c r="J26" t="s">
+        <v>623</v>
+      </c>
+      <c r="K26" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>620</v>
+      </c>
+      <c r="B27" t="s">
+        <v>660</v>
+      </c>
+      <c r="I27" t="s">
+        <v>621</v>
+      </c>
+      <c r="J27" t="s">
+        <v>621</v>
+      </c>
+      <c r="K27" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>632</v>
+      </c>
+      <c r="B28" t="s">
+        <v>661</v>
+      </c>
+      <c r="L28" t="s">
+        <v>627</v>
+      </c>
+      <c r="M28" t="s">
+        <v>627</v>
+      </c>
+      <c r="N28" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>633</v>
+      </c>
+      <c r="B29" t="s">
+        <v>662</v>
+      </c>
+      <c r="L29" t="s">
+        <v>628</v>
+      </c>
+      <c r="M29" t="s">
+        <v>628</v>
+      </c>
+      <c r="N29" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>635</v>
+      </c>
+      <c r="B30" t="s">
+        <v>664</v>
+      </c>
+      <c r="L30" t="s">
+        <v>629</v>
+      </c>
+      <c r="M30" t="s">
+        <v>629</v>
+      </c>
+      <c r="N30" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>634</v>
+      </c>
+      <c r="B31" t="s">
+        <v>663</v>
+      </c>
+      <c r="L31" t="s">
+        <v>630</v>
+      </c>
+      <c r="M31" t="s">
+        <v>630</v>
+      </c>
+      <c r="N31" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>593</v>
+      </c>
+      <c r="B32" t="s">
+        <v>665</v>
+      </c>
+      <c r="L32" t="s">
+        <v>631</v>
+      </c>
+      <c r="M32" t="s">
+        <v>631</v>
+      </c>
+      <c r="N32" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>803</v>
+      </c>
+      <c r="B33" t="s">
+        <v>808</v>
+      </c>
+      <c r="O33" t="s">
+        <v>804</v>
+      </c>
+      <c r="P33" t="s">
+        <v>804</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>805</v>
+      </c>
+      <c r="B34" t="s">
+        <v>809</v>
+      </c>
+      <c r="O34" t="s">
+        <v>806</v>
+      </c>
+      <c r="P34" t="s">
+        <v>806</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>806</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676CB143-3A50-44A7-AA3F-3DB79FFC4BAC}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D2" t="s">
+        <v>795</v>
+      </c>
+      <c r="E2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>741</v>
+      </c>
+      <c r="B3" t="s">
+        <v>669</v>
+      </c>
+      <c r="C3" t="s">
+        <v>669</v>
+      </c>
+      <c r="D3" t="s">
+        <v>669</v>
+      </c>
+      <c r="E3" t="s">
+        <v>670</v>
+      </c>
+      <c r="F3" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C4" t="s">
+        <v>728</v>
+      </c>
+      <c r="D4" t="s">
+        <v>728</v>
+      </c>
+      <c r="E4" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>763</v>
+      </c>
+      <c r="B5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C5" t="s">
+        <v>671</v>
+      </c>
+      <c r="D5" t="s">
+        <v>671</v>
+      </c>
+      <c r="E5" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>742</v>
+      </c>
+      <c r="B6" t="s">
+        <v>673</v>
+      </c>
+      <c r="C6" t="s">
+        <v>673</v>
+      </c>
+      <c r="D6" t="s">
+        <v>673</v>
+      </c>
+      <c r="E6" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>743</v>
+      </c>
+      <c r="B7" t="s">
+        <v>675</v>
+      </c>
+      <c r="C7" t="s">
+        <v>675</v>
+      </c>
+      <c r="D7" t="s">
+        <v>675</v>
+      </c>
+      <c r="E7" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>777</v>
+      </c>
+      <c r="C8" t="s">
+        <v>677</v>
+      </c>
+      <c r="D8" t="s">
+        <v>677</v>
+      </c>
+      <c r="E8" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>764</v>
+      </c>
+      <c r="B9" t="s">
+        <v>679</v>
+      </c>
+      <c r="C9" t="s">
+        <v>679</v>
+      </c>
+      <c r="D9" t="s">
+        <v>679</v>
+      </c>
+      <c r="E9" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>745</v>
+      </c>
+      <c r="C10" t="s">
+        <v>779</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="E10" t="s">
+        <v>744</v>
+      </c>
+      <c r="G10" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>747</v>
+      </c>
+      <c r="C11" t="s">
+        <v>681</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E11" t="s">
+        <v>746</v>
+      </c>
+      <c r="G11" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>749</v>
+      </c>
+      <c r="B12" t="s">
+        <v>682</v>
+      </c>
+      <c r="C12" t="s">
+        <v>682</v>
+      </c>
+      <c r="D12" t="s">
+        <v>682</v>
+      </c>
+      <c r="E12" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>748</v>
+      </c>
+      <c r="B13" t="s">
+        <v>684</v>
+      </c>
+      <c r="C13" t="s">
+        <v>684</v>
+      </c>
+      <c r="D13" t="s">
+        <v>684</v>
+      </c>
+      <c r="E13" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>766</v>
+      </c>
+      <c r="B14" t="s">
+        <v>686</v>
+      </c>
+      <c r="C14" t="s">
+        <v>686</v>
+      </c>
+      <c r="D14" t="s">
+        <v>686</v>
+      </c>
+      <c r="E14" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>750</v>
+      </c>
+      <c r="B15" t="s">
+        <v>688</v>
+      </c>
+      <c r="C15" t="s">
+        <v>688</v>
+      </c>
+      <c r="D15" t="s">
+        <v>688</v>
+      </c>
+      <c r="E15" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>751</v>
+      </c>
+      <c r="B16" t="s">
+        <v>690</v>
+      </c>
+      <c r="C16" t="s">
+        <v>690</v>
+      </c>
+      <c r="D16" t="s">
+        <v>794</v>
+      </c>
+      <c r="E16" t="s">
+        <v>691</v>
+      </c>
+      <c r="G16" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D17" t="s">
+        <v>698</v>
+      </c>
+      <c r="E17" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>767</v>
+      </c>
+      <c r="B18" t="s">
+        <v>692</v>
+      </c>
+      <c r="C18" t="s">
+        <v>692</v>
+      </c>
+      <c r="D18" t="s">
+        <v>692</v>
+      </c>
+      <c r="E18" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>752</v>
+      </c>
+      <c r="B19" t="s">
+        <v>694</v>
+      </c>
+      <c r="C19" t="s">
+        <v>694</v>
+      </c>
+      <c r="D19" t="s">
+        <v>694</v>
+      </c>
+      <c r="E19" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>753</v>
+      </c>
+      <c r="B20" t="s">
+        <v>696</v>
+      </c>
+      <c r="C20" t="s">
+        <v>696</v>
+      </c>
+      <c r="D20" t="s">
+        <v>696</v>
+      </c>
+      <c r="E20" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>776</v>
+      </c>
+      <c r="C21" t="s">
+        <v>699</v>
+      </c>
+      <c r="D21" t="s">
+        <v>699</v>
+      </c>
+      <c r="E21" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>768</v>
+      </c>
+      <c r="B22" t="s">
+        <v>701</v>
+      </c>
+      <c r="C22" t="s">
+        <v>701</v>
+      </c>
+      <c r="D22" t="s">
+        <v>701</v>
+      </c>
+      <c r="E22" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>754</v>
+      </c>
+      <c r="B23" t="s">
+        <v>703</v>
+      </c>
+      <c r="C23" t="s">
+        <v>703</v>
+      </c>
+      <c r="D23" t="s">
+        <v>703</v>
+      </c>
+      <c r="E23" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>756</v>
+      </c>
+      <c r="B24" t="s">
+        <v>705</v>
+      </c>
+      <c r="C24" t="s">
+        <v>705</v>
+      </c>
+      <c r="D24" t="s">
+        <v>705</v>
+      </c>
+      <c r="E24" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>755</v>
+      </c>
+      <c r="B25" t="s">
+        <v>707</v>
+      </c>
+      <c r="C25" t="s">
+        <v>707</v>
+      </c>
+      <c r="D25" t="s">
+        <v>707</v>
+      </c>
+      <c r="E25" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>757</v>
+      </c>
+      <c r="B26" t="s">
+        <v>709</v>
+      </c>
+      <c r="C26" t="s">
+        <v>709</v>
+      </c>
+      <c r="D26" t="s">
+        <v>709</v>
+      </c>
+      <c r="E26" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>758</v>
+      </c>
+      <c r="B27" t="s">
+        <v>711</v>
+      </c>
+      <c r="C27" t="s">
+        <v>711</v>
+      </c>
+      <c r="D27" t="s">
+        <v>711</v>
+      </c>
+      <c r="E27" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>765</v>
+      </c>
+      <c r="B28" t="s">
+        <v>713</v>
+      </c>
+      <c r="C28" t="s">
+        <v>713</v>
+      </c>
+      <c r="D28" t="s">
+        <v>810</v>
+      </c>
+      <c r="E28" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>769</v>
+      </c>
+      <c r="B29" t="s">
+        <v>717</v>
+      </c>
+      <c r="C29" t="s">
+        <v>715</v>
+      </c>
+      <c r="D29" t="s">
+        <v>715</v>
+      </c>
+      <c r="E29" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>771</v>
+      </c>
+      <c r="C30" t="s">
+        <v>718</v>
+      </c>
+      <c r="D30" t="s">
+        <v>718</v>
+      </c>
+      <c r="E30" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>770</v>
+      </c>
+      <c r="B31" t="s">
+        <v>720</v>
+      </c>
+      <c r="C31" t="s">
+        <v>720</v>
+      </c>
+      <c r="D31" t="s">
+        <v>720</v>
+      </c>
+      <c r="E31" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>772</v>
+      </c>
+      <c r="B32" t="s">
+        <v>722</v>
+      </c>
+      <c r="C32" t="s">
+        <v>722</v>
+      </c>
+      <c r="D32" t="s">
+        <v>722</v>
+      </c>
+      <c r="E32" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>759</v>
+      </c>
+      <c r="B33" t="s">
+        <v>724</v>
+      </c>
+      <c r="C33" t="s">
+        <v>724</v>
+      </c>
+      <c r="D33" t="s">
+        <v>724</v>
+      </c>
+      <c r="E33" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>773</v>
+      </c>
+      <c r="B34" t="s">
+        <v>726</v>
+      </c>
+      <c r="C34" t="s">
+        <v>726</v>
+      </c>
+      <c r="D34" t="s">
+        <v>726</v>
+      </c>
+      <c r="E34" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>761</v>
+      </c>
+      <c r="B35" t="s">
+        <v>730</v>
+      </c>
+      <c r="C35" t="s">
+        <v>730</v>
+      </c>
+      <c r="D35" t="s">
+        <v>730</v>
+      </c>
+      <c r="E35" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>774</v>
+      </c>
+      <c r="B36" t="s">
+        <v>732</v>
+      </c>
+      <c r="C36" t="s">
+        <v>732</v>
+      </c>
+      <c r="D36" t="s">
+        <v>732</v>
+      </c>
+      <c r="E36" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>775</v>
+      </c>
+      <c r="B37" t="s">
+        <v>736</v>
+      </c>
+      <c r="C37" t="s">
+        <v>734</v>
+      </c>
+      <c r="D37" t="s">
+        <v>734</v>
+      </c>
+      <c r="E37" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>762</v>
+      </c>
+      <c r="B38" t="s">
+        <v>737</v>
+      </c>
+      <c r="C38" t="s">
+        <v>737</v>
+      </c>
+      <c r="D38" t="s">
+        <v>737</v>
+      </c>
+      <c r="E38" t="s">
+        <v>738</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated S20 and added z-test
</commit_message>
<xml_diff>
--- a/data/mapping_ext.xlsx
+++ b/data/mapping_ext.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs-child-malnutrition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF344E5-C1BB-466C-A406-D2013A63AAC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74224C9-D744-4071-86F0-2F5709247836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25050" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25050" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nfhs5_state" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="814">
   <si>
     <t>ID</t>
   </si>
@@ -2471,6 +2471,15 @@
   </si>
   <si>
     <t>nct of delhi</t>
+  </si>
+  <si>
+    <t>Age at first marriage</t>
+  </si>
+  <si>
+    <t>s309</t>
+  </si>
+  <si>
+    <t>m_age1marriage</t>
   </si>
 </sst>
 </file>
@@ -9096,11 +9105,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF69C584-A901-4755-AAF5-5F5002664C77}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9817,239 +9826,253 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>609</v>
+        <v>811</v>
       </c>
       <c r="B21" t="s">
-        <v>654</v>
-      </c>
-      <c r="F21" t="s">
-        <v>597</v>
+        <v>813</v>
       </c>
       <c r="G21" t="s">
-        <v>597</v>
+        <v>812</v>
       </c>
       <c r="H21" t="s">
-        <v>597</v>
+        <v>812</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="B22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F22" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="G22" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="H22" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="B23" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F23" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="G23" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="H23" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B24" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F24" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="G24" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="H24" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B25" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F25" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G25" t="s">
-        <v>614</v>
+        <v>598</v>
       </c>
       <c r="H25" t="s">
-        <v>617</v>
+        <v>598</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B26" t="s">
-        <v>659</v>
-      </c>
-      <c r="I26" t="s">
-        <v>619</v>
-      </c>
-      <c r="J26" t="s">
-        <v>623</v>
-      </c>
-      <c r="K26" t="s">
-        <v>622</v>
+        <v>658</v>
+      </c>
+      <c r="F26" t="s">
+        <v>599</v>
+      </c>
+      <c r="G26" t="s">
+        <v>614</v>
+      </c>
+      <c r="H26" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="J27" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="K27" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="B28" t="s">
-        <v>661</v>
-      </c>
-      <c r="L28" t="s">
-        <v>627</v>
-      </c>
-      <c r="M28" t="s">
-        <v>627</v>
-      </c>
-      <c r="N28" t="s">
-        <v>627</v>
+        <v>660</v>
+      </c>
+      <c r="I28" t="s">
+        <v>621</v>
+      </c>
+      <c r="J28" t="s">
+        <v>621</v>
+      </c>
+      <c r="K28" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B29" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="L29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="M29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="N29" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B30" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="L30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="M30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="N30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B31" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="L31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="M31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="N31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
       <c r="B32" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="L32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="M32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="N32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>803</v>
+        <v>593</v>
       </c>
       <c r="B33" t="s">
-        <v>808</v>
-      </c>
-      <c r="O33" t="s">
-        <v>804</v>
-      </c>
-      <c r="P33" t="s">
-        <v>804</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>804</v>
+        <v>665</v>
+      </c>
+      <c r="L33" t="s">
+        <v>631</v>
+      </c>
+      <c r="M33" t="s">
+        <v>631</v>
+      </c>
+      <c r="N33" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>803</v>
+      </c>
+      <c r="B34" t="s">
+        <v>808</v>
+      </c>
+      <c r="O34" t="s">
+        <v>804</v>
+      </c>
+      <c r="P34" t="s">
+        <v>804</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>805</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>809</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O35" t="s">
         <v>806</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P35" t="s">
         <v>806</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="Q35" t="s">
         <v>806</v>
       </c>
     </row>
@@ -10062,7 +10085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676CB143-3A50-44A7-AA3F-3DB79FFC4BAC}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>